<commit_message>
added command to verify logs of a multi container pod
</commit_message>
<xml_diff>
--- a/k8s-cheetsheet.xlsx
+++ b/k8s-cheetsheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\learnings\K8s\kubernetes-cheetsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F924AD02-E6BA-4336-838F-B57D6192A3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388AB8EA-217A-47F0-A0CC-83C0FC2E49C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{4673813A-C8CA-4F5F-8F16-F5EA136FDB5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4673813A-C8CA-4F5F-8F16-F5EA136FDB5D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="commands" sheetId="1" r:id="rId1"/>
     <sheet name="imperative" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>How to check the logs of running pod?</t>
   </si>
@@ -221,6 +221,12 @@
   <si>
     <t>kubectl create deployment webapp --image kodekloud/webapp-color
 kubectl scale deployment webapp --replicas=3</t>
+  </si>
+  <si>
+    <t>How to verify logs of a multi-container pod?</t>
+  </si>
+  <si>
+    <t>kubectl logs -f webapp --all-containers=true</t>
   </si>
 </sst>
 </file>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63ACE3D7-9FDD-4919-8B64-625BA13E2A47}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,6 +833,14 @@
         <v>53</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -836,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D2AB0-ACC6-457A-B065-C77AACC8940F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>